<commit_message>
Renderizar Organigrama con StreamLit-Flow & corrección de la validación de jefes ya que le pedía un superior al ceo
</commit_message>
<xml_diff>
--- a/data/tst.xlsx
+++ b/data/tst.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft5167433-my.sharepoint.com/personal/mfuquene_tads_com_co/Documents/Escritorio/Organigrama KPIs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{564F41E0-5813-4ECD-BBF4-BF08FE283E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3938CDE-8259-4A10-8AEC-E3E9CB432029}"/>
+  <xr:revisionPtr revIDLastSave="316" documentId="13_ncr:1_{564F41E0-5813-4ECD-BBF4-BF08FE283E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AAF4A2B-29E4-4C6B-B7D9-A73CC4F1B668}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Organigrma" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KPIs!$A$1:$P$173</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2651" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="643">
   <si>
     <t>Indicador</t>
   </si>
@@ -1997,7 +1997,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2020,17 +2020,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2338,29 +2399,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P173"/>
   <sheetViews>
-    <sheetView topLeftCell="F149" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K173"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="44" customWidth="1"/>
-    <col min="15" max="15" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2410,7 +2471,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2460,7 +2521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2510,7 +2571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2560,7 +2621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2610,7 +2671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2660,7 +2721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2710,7 +2771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2760,7 +2821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2810,7 +2871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2860,7 +2921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2910,7 +2971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2960,7 +3021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3010,7 +3071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -3060,7 +3121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -3110,7 +3171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3160,7 +3221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -3210,7 +3271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -3260,7 +3321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -3310,7 +3371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -3360,7 +3421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -3410,7 +3471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -3460,7 +3521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3510,7 +3571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -3560,7 +3621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -3610,7 +3671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -3660,7 +3721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -3710,7 +3771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -3760,7 +3821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -3810,7 +3871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -3860,7 +3921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -3910,7 +3971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -3960,7 +4021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -4010,7 +4071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -4060,7 +4121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -4110,7 +4171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -4160,7 +4221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -4210,7 +4271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -4260,7 +4321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -4310,7 +4371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -4360,7 +4421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -4410,7 +4471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -4460,7 +4521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -4510,7 +4571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -4560,7 +4621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -4610,7 +4671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -4660,7 +4721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -4710,7 +4771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -4760,7 +4821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -4810,7 +4871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -4860,7 +4921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -4910,7 +4971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -4960,7 +5021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -5010,7 +5071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -5060,7 +5121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -5110,7 +5171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -5160,7 +5221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -5210,7 +5271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -5260,7 +5321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -5310,7 +5371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -5360,7 +5421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -5410,7 +5471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -5460,7 +5521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>39</v>
       </c>
@@ -5510,7 +5571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -5560,7 +5621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>40</v>
       </c>
@@ -5610,7 +5671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -5660,7 +5721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -5710,7 +5771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>47</v>
       </c>
@@ -5760,7 +5821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -5810,7 +5871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -5860,7 +5921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -5910,7 +5971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -5960,7 +6021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -6010,7 +6071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -6060,7 +6121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -6110,7 +6171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>40</v>
       </c>
@@ -6160,7 +6221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -6210,7 +6271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -6260,7 +6321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>75</v>
       </c>
@@ -6310,7 +6371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -6360,7 +6421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -6410,7 +6471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -6460,7 +6521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -6510,7 +6571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -6560,7 +6621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -6610,7 +6671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>38</v>
       </c>
@@ -6660,7 +6721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>53</v>
       </c>
@@ -6710,7 +6771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>40</v>
       </c>
@@ -6760,7 +6821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>82</v>
       </c>
@@ -6810,7 +6871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>83</v>
       </c>
@@ -6860,7 +6921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>84</v>
       </c>
@@ -6910,7 +6971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>85</v>
       </c>
@@ -6960,7 +7021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>86</v>
       </c>
@@ -7010,7 +7071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>74</v>
       </c>
@@ -7060,7 +7121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>79</v>
       </c>
@@ -7110,7 +7171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>40</v>
       </c>
@@ -7160,7 +7221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>78</v>
       </c>
@@ -7210,7 +7271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>61</v>
       </c>
@@ -7260,7 +7321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -7310,7 +7371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>88</v>
       </c>
@@ -7360,7 +7421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>89</v>
       </c>
@@ -7410,7 +7471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -7460,7 +7521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>91</v>
       </c>
@@ -7510,7 +7571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>92</v>
       </c>
@@ -7560,7 +7621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>93</v>
       </c>
@@ -7610,7 +7671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>94</v>
       </c>
@@ -7660,7 +7721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>95</v>
       </c>
@@ -7710,7 +7771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>96</v>
       </c>
@@ -7760,7 +7821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>70</v>
       </c>
@@ -7810,7 +7871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>83</v>
       </c>
@@ -7860,7 +7921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>97</v>
       </c>
@@ -7910,7 +7971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>75</v>
       </c>
@@ -7960,7 +8021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>86</v>
       </c>
@@ -8010,7 +8071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>71</v>
       </c>
@@ -8060,7 +8121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>72</v>
       </c>
@@ -8110,7 +8171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>98</v>
       </c>
@@ -8160,7 +8221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>99</v>
       </c>
@@ -8210,7 +8271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>100</v>
       </c>
@@ -8260,7 +8321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>35</v>
       </c>
@@ -8310,7 +8371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>101</v>
       </c>
@@ -8360,7 +8421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>102</v>
       </c>
@@ -8410,7 +8471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>71</v>
       </c>
@@ -8460,7 +8521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>72</v>
       </c>
@@ -8510,7 +8571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>103</v>
       </c>
@@ -8560,7 +8621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>43</v>
       </c>
@@ -8610,7 +8671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>101</v>
       </c>
@@ -8660,7 +8721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>100</v>
       </c>
@@ -8710,7 +8771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>40</v>
       </c>
@@ -8760,7 +8821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>41</v>
       </c>
@@ -8810,7 +8871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>104</v>
       </c>
@@ -8860,7 +8921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>105</v>
       </c>
@@ -8910,7 +8971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>46</v>
       </c>
@@ -8960,7 +9021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>106</v>
       </c>
@@ -9010,7 +9071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>104</v>
       </c>
@@ -9060,7 +9121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>46</v>
       </c>
@@ -9110,7 +9171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>107</v>
       </c>
@@ -9160,7 +9221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>108</v>
       </c>
@@ -9210,7 +9271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>32</v>
       </c>
@@ -9260,7 +9321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>33</v>
       </c>
@@ -9310,7 +9371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>109</v>
       </c>
@@ -9360,7 +9421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>110</v>
       </c>
@@ -9410,7 +9471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>111</v>
       </c>
@@ -9460,7 +9521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>112</v>
       </c>
@@ -9510,7 +9571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>113</v>
       </c>
@@ -9560,7 +9621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>114</v>
       </c>
@@ -9610,7 +9671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>83</v>
       </c>
@@ -9660,7 +9721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>115</v>
       </c>
@@ -9710,7 +9771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>80</v>
       </c>
@@ -9761,7 +9822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>116</v>
       </c>
@@ -9811,7 +9872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>117</v>
       </c>
@@ -9861,7 +9922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>87</v>
       </c>
@@ -9911,7 +9972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>118</v>
       </c>
@@ -9961,7 +10022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>119</v>
       </c>
@@ -10011,7 +10072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>120</v>
       </c>
@@ -10061,7 +10122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>53</v>
       </c>
@@ -10111,7 +10172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>40</v>
       </c>
@@ -10161,7 +10222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>121</v>
       </c>
@@ -10211,7 +10272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>122</v>
       </c>
@@ -10261,7 +10322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>123</v>
       </c>
@@ -10311,7 +10372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>124</v>
       </c>
@@ -10361,7 +10422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>125</v>
       </c>
@@ -10411,7 +10472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>122</v>
       </c>
@@ -10461,7 +10522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>126</v>
       </c>
@@ -10511,7 +10572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>127</v>
       </c>
@@ -10561,7 +10622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>128</v>
       </c>
@@ -10611,7 +10672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>30</v>
       </c>
@@ -10661,7 +10722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>52</v>
       </c>
@@ -10711,7 +10772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>129</v>
       </c>
@@ -10761,7 +10822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>130</v>
       </c>
@@ -10811,7 +10872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>90</v>
       </c>
@@ -10861,7 +10922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>80</v>
       </c>
@@ -10911,7 +10972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>131</v>
       </c>
@@ -10961,7 +11022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>132</v>
       </c>
@@ -11018,247 +11079,345 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04227A6E-AE07-4A2E-B2E3-937F699C5555}">
-  <dimension ref="A1:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A9EAA1-EB7F-45F3-BA80-95884B8E9BF8}">
+  <dimension ref="B2:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="2"/>
+    <col min="2" max="2" width="27.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="10"/>
+      <c r="C8" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="10"/>
+      <c r="C11" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="10"/>
+      <c r="C12" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="C15" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="6"/>
+      <c r="C31" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="6"/>
+      <c r="C38" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="6"/>
+      <c r="C39" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="6"/>
+      <c r="C40" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="6"/>
+      <c r="C43" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>460</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>461</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>352</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>353</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>354</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>450</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>437</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>459</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C45" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="6"/>
+      <c r="C46" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>469</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>363</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>366</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C52" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>463</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>455</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>464</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>452</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>465</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>471</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C56" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>468</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>456</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>462</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>458</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>473</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>457</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="C60" s="3" t="s">
         <v>385</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A28">
-    <sortCondition ref="A1:A28"/>
-  </sortState>
+  <mergeCells count="9">
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B37:B40"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificaciones semana 11 al 14 de noviembre
</commit_message>
<xml_diff>
--- a/data/tst.xlsx
+++ b/data/tst.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft5167433-my.sharepoint.com/personal/mfuquene_tads_com_co/Documents/Escritorio/Organigrama KPIs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="13_ncr:1_{564F41E0-5813-4ECD-BBF4-BF08FE283E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AAF4A2B-29E4-4C6B-B7D9-A73CC4F1B668}"/>
+  <xr:revisionPtr revIDLastSave="322" documentId="13_ncr:1_{564F41E0-5813-4ECD-BBF4-BF08FE283E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB53413B-82FA-4D94-8CD8-49D86323883D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="642">
   <si>
     <t>Indicador</t>
   </si>
@@ -1480,9 +1480,6 @@
   </si>
   <si>
     <t>Gerente</t>
-  </si>
-  <si>
-    <t>Asistente/Auxiliar</t>
   </si>
   <si>
     <t>Satisfacción del cliente</t>
@@ -2061,7 +2058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2093,6 +2090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2397,31 +2395,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P173"/>
+    <sheetView tabSelected="1" topLeftCell="F50" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50:L169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="44" customWidth="1"/>
-    <col min="15" max="15" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2468,10 +2467,10 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2509,19 +2508,19 @@
         <v>475</v>
       </c>
       <c r="M2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2559,19 +2558,19 @@
         <v>475</v>
       </c>
       <c r="M3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="O3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2609,19 +2608,19 @@
         <v>475</v>
       </c>
       <c r="M4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="O4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2659,19 +2658,19 @@
         <v>475</v>
       </c>
       <c r="M5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2709,19 +2708,19 @@
         <v>476</v>
       </c>
       <c r="M6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2759,19 +2758,19 @@
         <v>476</v>
       </c>
       <c r="M7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2809,19 +2808,19 @@
         <v>476</v>
       </c>
       <c r="M8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N8" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="O8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2859,19 +2858,19 @@
         <v>476</v>
       </c>
       <c r="M9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="O9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2909,19 +2908,19 @@
         <v>476</v>
       </c>
       <c r="M10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2959,19 +2958,19 @@
         <v>476</v>
       </c>
       <c r="M11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N11" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="O11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -3009,19 +3008,19 @@
         <v>476</v>
       </c>
       <c r="M12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="O12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3059,19 +3058,19 @@
         <v>476</v>
       </c>
       <c r="M13" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N13" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="O13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -3109,19 +3108,19 @@
         <v>476</v>
       </c>
       <c r="M14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N14" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="O14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P14">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -3159,19 +3158,19 @@
         <v>476</v>
       </c>
       <c r="M15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N15" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="O15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3209,19 +3208,19 @@
         <v>476</v>
       </c>
       <c r="M16" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N16" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="O16" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P16">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -3259,19 +3258,19 @@
         <v>476</v>
       </c>
       <c r="M17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N17" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="O17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -3309,19 +3308,19 @@
         <v>476</v>
       </c>
       <c r="M18" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N18" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="O18" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -3359,19 +3358,19 @@
         <v>476</v>
       </c>
       <c r="M19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="O19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -3409,19 +3408,19 @@
         <v>476</v>
       </c>
       <c r="M20" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="O20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P20">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -3459,19 +3458,19 @@
         <v>476</v>
       </c>
       <c r="M21" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="O21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P21">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -3509,19 +3508,19 @@
         <v>476</v>
       </c>
       <c r="M22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N22" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="O22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P22">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3559,19 +3558,19 @@
         <v>476</v>
       </c>
       <c r="M23" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N23" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="O23" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P23">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -3609,19 +3608,19 @@
         <v>476</v>
       </c>
       <c r="M24" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="O24" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P24">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -3659,19 +3658,19 @@
         <v>476</v>
       </c>
       <c r="M25" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="O25" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -3709,19 +3708,19 @@
         <v>477</v>
       </c>
       <c r="M26" t="s">
+        <v>483</v>
+      </c>
+      <c r="N26" t="s">
+        <v>511</v>
+      </c>
+      <c r="O26" t="s">
         <v>484</v>
       </c>
-      <c r="N26" t="s">
-        <v>512</v>
-      </c>
-      <c r="O26" t="s">
-        <v>485</v>
-      </c>
       <c r="P26">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -3759,19 +3758,19 @@
         <v>477</v>
       </c>
       <c r="M27" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N27" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="O27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P27">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -3809,19 +3808,19 @@
         <v>477</v>
       </c>
       <c r="M28" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="O28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P28">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -3859,19 +3858,19 @@
         <v>477</v>
       </c>
       <c r="M29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N29" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="O29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="P29">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -3909,19 +3908,19 @@
         <v>477</v>
       </c>
       <c r="M30" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N30" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="O30" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P30">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>437</v>
       </c>
       <c r="L31" t="s">
-        <v>346</v>
+        <v>476</v>
       </c>
       <c r="M31" t="s">
         <v>460</v>
@@ -3965,13 +3964,13 @@
         <v>477</v>
       </c>
       <c r="O31" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P31">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -4009,19 +4008,19 @@
         <v>477</v>
       </c>
       <c r="M32" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="O32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P32">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -4059,19 +4058,19 @@
         <v>477</v>
       </c>
       <c r="M33" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="O33" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P33">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -4109,19 +4108,19 @@
         <v>477</v>
       </c>
       <c r="M34" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N34" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O34" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P34">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -4159,19 +4158,19 @@
         <v>477</v>
       </c>
       <c r="M35" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N35" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="O35" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P35">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -4209,19 +4208,19 @@
         <v>477</v>
       </c>
       <c r="M36" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N36" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O36" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P36">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -4259,19 +4258,19 @@
         <v>477</v>
       </c>
       <c r="M37" t="s">
+        <v>483</v>
+      </c>
+      <c r="N37" t="s">
+        <v>520</v>
+      </c>
+      <c r="O37" t="s">
         <v>484</v>
       </c>
-      <c r="N37" t="s">
-        <v>521</v>
-      </c>
-      <c r="O37" t="s">
-        <v>485</v>
-      </c>
       <c r="P37">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -4309,19 +4308,19 @@
         <v>477</v>
       </c>
       <c r="M38" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N38" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="O38" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P38">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -4359,19 +4358,19 @@
         <v>477</v>
       </c>
       <c r="M39" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N39" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O39" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P39">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -4409,19 +4408,19 @@
         <v>477</v>
       </c>
       <c r="M40" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N40" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="O40" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P40">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -4459,19 +4458,19 @@
         <v>477</v>
       </c>
       <c r="M41" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N41" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="O41" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P41">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -4509,19 +4508,19 @@
         <v>477</v>
       </c>
       <c r="M42" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N42" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="O42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P42">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -4559,19 +4558,19 @@
         <v>477</v>
       </c>
       <c r="M43" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N43" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="O43" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P43">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -4609,19 +4608,19 @@
         <v>477</v>
       </c>
       <c r="M44" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N44" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="O44" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P44">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -4659,19 +4658,19 @@
         <v>477</v>
       </c>
       <c r="M45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N45" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="O45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P45">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -4709,19 +4708,19 @@
         <v>477</v>
       </c>
       <c r="M46" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N46" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="O46" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P46">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -4759,19 +4758,19 @@
         <v>477</v>
       </c>
       <c r="M47" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="O47" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P47">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -4809,19 +4808,19 @@
         <v>477</v>
       </c>
       <c r="M48" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N48" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="O48" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P48">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -4859,19 +4858,19 @@
         <v>477</v>
       </c>
       <c r="M49" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N49" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="O49" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P49">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -4905,23 +4904,23 @@
       <c r="K50" t="s">
         <v>464</v>
       </c>
-      <c r="L50" t="s">
+      <c r="L50" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M50" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N50" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="O50" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P50">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -4955,23 +4954,23 @@
       <c r="K51" t="s">
         <v>464</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L51" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M51" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N51" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="O51" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P51">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -5005,23 +5004,23 @@
       <c r="K52" t="s">
         <v>464</v>
       </c>
-      <c r="L52" t="s">
+      <c r="L52" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M52" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N52" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="O52" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P52">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -5055,23 +5054,23 @@
       <c r="K53" t="s">
         <v>464</v>
       </c>
-      <c r="L53" t="s">
+      <c r="L53" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M53" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N53" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O53" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P53">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -5105,23 +5104,23 @@
       <c r="K54" t="s">
         <v>465</v>
       </c>
-      <c r="L54" t="s">
+      <c r="L54" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M54" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N54" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="O54" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P54">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -5155,23 +5154,23 @@
       <c r="K55" t="s">
         <v>465</v>
       </c>
-      <c r="L55" t="s">
+      <c r="L55" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M55" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N55" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="O55" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P55">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -5205,23 +5204,23 @@
       <c r="K56" t="s">
         <v>465</v>
       </c>
-      <c r="L56" t="s">
+      <c r="L56" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M56" t="s">
+        <v>483</v>
+      </c>
+      <c r="N56" t="s">
+        <v>539</v>
+      </c>
+      <c r="O56" t="s">
         <v>484</v>
       </c>
-      <c r="N56" t="s">
-        <v>540</v>
-      </c>
-      <c r="O56" t="s">
-        <v>485</v>
-      </c>
       <c r="P56">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -5255,23 +5254,23 @@
       <c r="K57" t="s">
         <v>465</v>
       </c>
-      <c r="L57" t="s">
+      <c r="L57" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M57" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N57" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="O57" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P57">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -5309,19 +5308,19 @@
         <v>451</v>
       </c>
       <c r="M58" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N58" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="O58" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P58">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -5359,19 +5358,19 @@
         <v>451</v>
       </c>
       <c r="M59" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N59" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="O59" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P59">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -5409,19 +5408,19 @@
         <v>451</v>
       </c>
       <c r="M60" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N60" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="O60" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P60">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -5459,19 +5458,19 @@
         <v>451</v>
       </c>
       <c r="M61" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N61" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="O61" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P61">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -5509,19 +5508,19 @@
         <v>451</v>
       </c>
       <c r="M62" t="s">
+        <v>483</v>
+      </c>
+      <c r="N62" t="s">
+        <v>545</v>
+      </c>
+      <c r="O62" t="s">
         <v>484</v>
       </c>
-      <c r="N62" t="s">
-        <v>546</v>
-      </c>
-      <c r="O62" t="s">
-        <v>485</v>
-      </c>
       <c r="P62">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>39</v>
       </c>
@@ -5559,19 +5558,19 @@
         <v>451</v>
       </c>
       <c r="M63" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N63" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="O63" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P63">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -5609,19 +5608,19 @@
         <v>451</v>
       </c>
       <c r="M64" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N64" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="O64" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P64">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>40</v>
       </c>
@@ -5659,19 +5658,19 @@
         <v>451</v>
       </c>
       <c r="M65" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N65" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="O65" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P65">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -5709,19 +5708,19 @@
         <v>451</v>
       </c>
       <c r="M66" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N66" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="O66" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P66">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -5759,19 +5758,19 @@
         <v>451</v>
       </c>
       <c r="M67" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N67" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="O67" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P67">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>47</v>
       </c>
@@ -5809,19 +5808,19 @@
         <v>451</v>
       </c>
       <c r="M68" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N68" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="O68" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P68">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -5859,19 +5858,19 @@
         <v>451</v>
       </c>
       <c r="M69" t="s">
+        <v>483</v>
+      </c>
+      <c r="N69" t="s">
+        <v>551</v>
+      </c>
+      <c r="O69" t="s">
         <v>484</v>
       </c>
-      <c r="N69" t="s">
-        <v>552</v>
-      </c>
-      <c r="O69" t="s">
-        <v>485</v>
-      </c>
       <c r="P69">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -5909,19 +5908,19 @@
         <v>451</v>
       </c>
       <c r="M70" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N70" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="O70" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P70">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -5959,19 +5958,19 @@
         <v>451</v>
       </c>
       <c r="M71" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N71" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="O71" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P71">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -6009,19 +6008,19 @@
         <v>451</v>
       </c>
       <c r="M72" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N72" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="O72" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P72">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -6059,19 +6058,19 @@
         <v>451</v>
       </c>
       <c r="M73" t="s">
+        <v>483</v>
+      </c>
+      <c r="N73" t="s">
+        <v>555</v>
+      </c>
+      <c r="O73" t="s">
         <v>484</v>
       </c>
-      <c r="N73" t="s">
-        <v>556</v>
-      </c>
-      <c r="O73" t="s">
-        <v>485</v>
-      </c>
       <c r="P73">
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -6109,19 +6108,19 @@
         <v>451</v>
       </c>
       <c r="M74" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N74" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="O74" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P74">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -6159,19 +6158,19 @@
         <v>451</v>
       </c>
       <c r="M75" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N75" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="O75" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P75">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>40</v>
       </c>
@@ -6209,19 +6208,19 @@
         <v>451</v>
       </c>
       <c r="M76" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N76" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="O76" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P76">
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -6259,19 +6258,19 @@
         <v>451</v>
       </c>
       <c r="M77" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N77" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O77" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P77">
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -6309,19 +6308,19 @@
         <v>451</v>
       </c>
       <c r="M78" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N78" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="O78" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P78">
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>75</v>
       </c>
@@ -6359,19 +6358,19 @@
         <v>451</v>
       </c>
       <c r="M79" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N79" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="O79" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P79">
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -6409,19 +6408,19 @@
         <v>451</v>
       </c>
       <c r="M80" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N80" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="O80" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P80">
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -6459,19 +6458,19 @@
         <v>451</v>
       </c>
       <c r="M81" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N81" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="O81" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P81">
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -6509,19 +6508,19 @@
         <v>451</v>
       </c>
       <c r="M82" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N82" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="O82" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P82">
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -6559,19 +6558,19 @@
         <v>451</v>
       </c>
       <c r="M83" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N83" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="O83" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P83">
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -6609,19 +6608,19 @@
         <v>451</v>
       </c>
       <c r="M84" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N84" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="O84" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P84">
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -6659,19 +6658,19 @@
         <v>451</v>
       </c>
       <c r="M85" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N85" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="O85" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P85">
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>38</v>
       </c>
@@ -6705,23 +6704,23 @@
       <c r="K86" t="s">
         <v>353</v>
       </c>
-      <c r="L86" t="s">
+      <c r="L86" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M86" t="s">
+        <v>483</v>
+      </c>
+      <c r="N86" t="s">
+        <v>545</v>
+      </c>
+      <c r="O86" t="s">
         <v>484</v>
       </c>
-      <c r="N86" t="s">
-        <v>546</v>
-      </c>
-      <c r="O86" t="s">
-        <v>485</v>
-      </c>
       <c r="P86">
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>53</v>
       </c>
@@ -6755,23 +6754,23 @@
       <c r="K87" t="s">
         <v>353</v>
       </c>
-      <c r="L87" t="s">
+      <c r="L87" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M87" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N87" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="O87" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P87">
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>40</v>
       </c>
@@ -6805,23 +6804,23 @@
       <c r="K88" t="s">
         <v>353</v>
       </c>
-      <c r="L88" t="s">
+      <c r="L88" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M88" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N88" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="O88" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P88">
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>82</v>
       </c>
@@ -6855,23 +6854,23 @@
       <c r="K89" t="s">
         <v>353</v>
       </c>
-      <c r="L89" t="s">
+      <c r="L89" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M89" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N89" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="O89" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="P89">
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>83</v>
       </c>
@@ -6909,19 +6908,19 @@
         <v>479</v>
       </c>
       <c r="M90" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N90" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="O90" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P90">
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>84</v>
       </c>
@@ -6959,19 +6958,19 @@
         <v>479</v>
       </c>
       <c r="M91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N91" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="O91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P91">
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>85</v>
       </c>
@@ -7009,19 +7008,19 @@
         <v>479</v>
       </c>
       <c r="M92" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N92" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="O92" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P92">
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>86</v>
       </c>
@@ -7059,19 +7058,19 @@
         <v>479</v>
       </c>
       <c r="M93" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N93" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="O93" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P93">
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>74</v>
       </c>
@@ -7109,19 +7108,19 @@
         <v>480</v>
       </c>
       <c r="M94" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N94" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="O94" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P94">
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>79</v>
       </c>
@@ -7159,19 +7158,19 @@
         <v>480</v>
       </c>
       <c r="M95" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N95" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="O95" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P95">
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>40</v>
       </c>
@@ -7209,19 +7208,19 @@
         <v>480</v>
       </c>
       <c r="M96" t="s">
+        <v>483</v>
+      </c>
+      <c r="N96" t="s">
+        <v>575</v>
+      </c>
+      <c r="O96" t="s">
         <v>484</v>
       </c>
-      <c r="N96" t="s">
-        <v>576</v>
-      </c>
-      <c r="O96" t="s">
-        <v>485</v>
-      </c>
       <c r="P96">
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>78</v>
       </c>
@@ -7259,19 +7258,19 @@
         <v>480</v>
       </c>
       <c r="M97" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N97" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="O97" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P97">
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>61</v>
       </c>
@@ -7309,19 +7308,19 @@
         <v>475</v>
       </c>
       <c r="M98" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N98" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="O98" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P98">
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -7359,19 +7358,19 @@
         <v>475</v>
       </c>
       <c r="M99" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N99" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="O99" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P99">
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>88</v>
       </c>
@@ -7409,19 +7408,19 @@
         <v>475</v>
       </c>
       <c r="M100" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N100" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="O100" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P100">
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>89</v>
       </c>
@@ -7459,19 +7458,19 @@
         <v>475</v>
       </c>
       <c r="M101" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N101" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="O101" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P101">
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -7509,19 +7508,19 @@
         <v>475</v>
       </c>
       <c r="M102" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N102" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="O102" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P102">
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>91</v>
       </c>
@@ -7559,19 +7558,19 @@
         <v>475</v>
       </c>
       <c r="M103" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N103" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="O103" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P103">
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>92</v>
       </c>
@@ -7609,19 +7608,19 @@
         <v>475</v>
       </c>
       <c r="M104" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N104" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="O104" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P104">
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>93</v>
       </c>
@@ -7659,19 +7658,19 @@
         <v>475</v>
       </c>
       <c r="M105" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N105" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="O105" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P105">
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>94</v>
       </c>
@@ -7709,19 +7708,19 @@
         <v>475</v>
       </c>
       <c r="M106" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N106" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="O106" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P106">
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>95</v>
       </c>
@@ -7759,19 +7758,19 @@
         <v>475</v>
       </c>
       <c r="M107" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N107" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="O107" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P107">
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>96</v>
       </c>
@@ -7809,19 +7808,19 @@
         <v>475</v>
       </c>
       <c r="M108" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N108" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="O108" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P108">
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>70</v>
       </c>
@@ -7859,19 +7858,19 @@
         <v>475</v>
       </c>
       <c r="M109" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N109" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="O109" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P109">
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>83</v>
       </c>
@@ -7909,19 +7908,19 @@
         <v>475</v>
       </c>
       <c r="M110" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N110" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="O110" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P110">
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>97</v>
       </c>
@@ -7959,19 +7958,19 @@
         <v>475</v>
       </c>
       <c r="M111" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N111" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="O111" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P111">
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>75</v>
       </c>
@@ -8009,19 +8008,19 @@
         <v>475</v>
       </c>
       <c r="M112" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N112" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="O112" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P112">
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>86</v>
       </c>
@@ -8059,19 +8058,19 @@
         <v>475</v>
       </c>
       <c r="M113" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N113" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="O113" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P113">
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>71</v>
       </c>
@@ -8105,23 +8104,23 @@
       <c r="K114" t="s">
         <v>467</v>
       </c>
-      <c r="L114" t="s">
+      <c r="L114" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M114" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N114" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="O114" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P114">
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>72</v>
       </c>
@@ -8155,23 +8154,23 @@
       <c r="K115" t="s">
         <v>467</v>
       </c>
-      <c r="L115" t="s">
+      <c r="L115" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M115" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N115" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="O115" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P115">
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>98</v>
       </c>
@@ -8205,23 +8204,23 @@
       <c r="K116" t="s">
         <v>467</v>
       </c>
-      <c r="L116" t="s">
+      <c r="L116" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M116" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N116" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="O116" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P116">
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>99</v>
       </c>
@@ -8255,23 +8254,23 @@
       <c r="K117" t="s">
         <v>467</v>
       </c>
-      <c r="L117" t="s">
+      <c r="L117" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M117" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N117" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="O117" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P117">
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>100</v>
       </c>
@@ -8305,23 +8304,23 @@
       <c r="K118" t="s">
         <v>464</v>
       </c>
-      <c r="L118" t="s">
+      <c r="L118" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M118" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N118" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="O118" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P118">
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>35</v>
       </c>
@@ -8355,23 +8354,23 @@
       <c r="K119" t="s">
         <v>464</v>
       </c>
-      <c r="L119" t="s">
+      <c r="L119" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M119" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N119" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="O119" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P119">
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>101</v>
       </c>
@@ -8405,23 +8404,23 @@
       <c r="K120" t="s">
         <v>464</v>
       </c>
-      <c r="L120" t="s">
+      <c r="L120" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M120" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N120" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="O120" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P120">
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>102</v>
       </c>
@@ -8455,23 +8454,23 @@
       <c r="K121" t="s">
         <v>464</v>
       </c>
-      <c r="L121" t="s">
+      <c r="L121" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M121" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N121" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="O121" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P121">
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>71</v>
       </c>
@@ -8505,23 +8504,23 @@
       <c r="K122" t="s">
         <v>464</v>
       </c>
-      <c r="L122" t="s">
+      <c r="L122" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M122" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N122" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O122" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P122">
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>72</v>
       </c>
@@ -8555,23 +8554,23 @@
       <c r="K123" t="s">
         <v>464</v>
       </c>
-      <c r="L123" t="s">
+      <c r="L123" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M123" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N123" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="O123" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P123">
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>103</v>
       </c>
@@ -8605,23 +8604,23 @@
       <c r="K124" t="s">
         <v>464</v>
       </c>
-      <c r="L124" t="s">
+      <c r="L124" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M124" t="s">
+        <v>483</v>
+      </c>
+      <c r="N124" t="s">
+        <v>601</v>
+      </c>
+      <c r="O124" t="s">
         <v>484</v>
       </c>
-      <c r="N124" t="s">
-        <v>602</v>
-      </c>
-      <c r="O124" t="s">
-        <v>485</v>
-      </c>
       <c r="P124">
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>43</v>
       </c>
@@ -8655,8 +8654,8 @@
       <c r="K125" t="s">
         <v>437</v>
       </c>
-      <c r="L125" t="s">
-        <v>373</v>
+      <c r="L125" s="11" t="s">
+        <v>478</v>
       </c>
       <c r="M125" t="s">
         <v>464</v>
@@ -8665,13 +8664,13 @@
         <v>478</v>
       </c>
       <c r="O125" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P125">
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>101</v>
       </c>
@@ -8705,23 +8704,23 @@
       <c r="K126" t="s">
         <v>464</v>
       </c>
-      <c r="L126" t="s">
+      <c r="L126" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M126" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N126" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="O126" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P126">
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>100</v>
       </c>
@@ -8755,23 +8754,23 @@
       <c r="K127" t="s">
         <v>464</v>
       </c>
-      <c r="L127" t="s">
+      <c r="L127" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M127" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N127" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O127" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P127">
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>40</v>
       </c>
@@ -8805,23 +8804,23 @@
       <c r="K128" t="s">
         <v>464</v>
       </c>
-      <c r="L128" t="s">
+      <c r="L128" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M128" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N128" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O128" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P128">
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>41</v>
       </c>
@@ -8855,23 +8854,23 @@
       <c r="K129" t="s">
         <v>464</v>
       </c>
-      <c r="L129" t="s">
+      <c r="L129" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M129" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N129" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="O129" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="P129">
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>104</v>
       </c>
@@ -8905,23 +8904,23 @@
       <c r="K130" t="s">
         <v>462</v>
       </c>
-      <c r="L130" t="s">
+      <c r="L130" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M130" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N130" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="O130" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P130">
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>105</v>
       </c>
@@ -8955,23 +8954,23 @@
       <c r="K131" t="s">
         <v>462</v>
       </c>
-      <c r="L131" t="s">
+      <c r="L131" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M131" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N131" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O131" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P131">
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>46</v>
       </c>
@@ -9005,23 +9004,23 @@
       <c r="K132" t="s">
         <v>462</v>
       </c>
-      <c r="L132" t="s">
+      <c r="L132" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M132" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N132" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="O132" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P132">
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>106</v>
       </c>
@@ -9055,23 +9054,23 @@
       <c r="K133" t="s">
         <v>462</v>
       </c>
-      <c r="L133" t="s">
+      <c r="L133" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M133" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N133" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="O133" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P133">
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>104</v>
       </c>
@@ -9105,23 +9104,23 @@
       <c r="K134" t="s">
         <v>470</v>
       </c>
-      <c r="L134" t="s">
+      <c r="L134" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M134" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N134" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="O134" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P134">
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>46</v>
       </c>
@@ -9155,23 +9154,23 @@
       <c r="K135" t="s">
         <v>470</v>
       </c>
-      <c r="L135" t="s">
+      <c r="L135" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M135" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N135" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="O135" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P135">
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>107</v>
       </c>
@@ -9205,23 +9204,23 @@
       <c r="K136" t="s">
         <v>470</v>
       </c>
-      <c r="L136" t="s">
+      <c r="L136" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M136" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N136" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="O136" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P136">
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>108</v>
       </c>
@@ -9255,23 +9254,23 @@
       <c r="K137" t="s">
         <v>470</v>
       </c>
-      <c r="L137" t="s">
+      <c r="L137" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M137" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N137" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="O137" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P137">
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>32</v>
       </c>
@@ -9305,23 +9304,23 @@
       <c r="K138" t="s">
         <v>455</v>
       </c>
-      <c r="L138" t="s">
+      <c r="L138" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M138" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N138" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="O138" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P138">
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>33</v>
       </c>
@@ -9355,23 +9354,23 @@
       <c r="K139" t="s">
         <v>455</v>
       </c>
-      <c r="L139" t="s">
+      <c r="L139" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M139" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N139" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="O139" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P139">
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>109</v>
       </c>
@@ -9405,23 +9404,23 @@
       <c r="K140" t="s">
         <v>455</v>
       </c>
-      <c r="L140" t="s">
+      <c r="L140" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M140" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N140" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="O140" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P140">
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>110</v>
       </c>
@@ -9455,23 +9454,23 @@
       <c r="K141" t="s">
         <v>455</v>
       </c>
-      <c r="L141" t="s">
+      <c r="L141" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M141" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N141" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="O141" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P141">
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>111</v>
       </c>
@@ -9505,23 +9504,23 @@
       <c r="K142" t="s">
         <v>471</v>
       </c>
-      <c r="L142" t="s">
+      <c r="L142" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M142" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N142" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="O142" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P142">
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>112</v>
       </c>
@@ -9555,23 +9554,23 @@
       <c r="K143" t="s">
         <v>471</v>
       </c>
-      <c r="L143" t="s">
+      <c r="L143" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M143" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N143" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="O143" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P143">
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>113</v>
       </c>
@@ -9605,23 +9604,23 @@
       <c r="K144" t="s">
         <v>471</v>
       </c>
-      <c r="L144" t="s">
+      <c r="L144" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M144" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N144" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="O144" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P144">
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>114</v>
       </c>
@@ -9655,23 +9654,23 @@
       <c r="K145" t="s">
         <v>471</v>
       </c>
-      <c r="L145" t="s">
+      <c r="L145" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M145" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N145" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="O145" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P145">
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>83</v>
       </c>
@@ -9705,23 +9704,23 @@
       <c r="K146" t="s">
         <v>472</v>
       </c>
-      <c r="L146" t="s">
+      <c r="L146" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M146" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N146" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="O146" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P146">
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>115</v>
       </c>
@@ -9755,23 +9754,23 @@
       <c r="K147" t="s">
         <v>472</v>
       </c>
-      <c r="L147" t="s">
+      <c r="L147" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M147" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N147" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="O147" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P147">
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>80</v>
       </c>
@@ -9806,23 +9805,23 @@
       <c r="K148" t="s">
         <v>472</v>
       </c>
-      <c r="L148" t="s">
+      <c r="L148" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M148" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N148" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="O148" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P148">
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>116</v>
       </c>
@@ -9856,23 +9855,23 @@
       <c r="K149" t="s">
         <v>472</v>
       </c>
-      <c r="L149" t="s">
+      <c r="L149" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M149" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N149" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="O149" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P149">
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>117</v>
       </c>
@@ -9906,23 +9905,23 @@
       <c r="K150" t="s">
         <v>465</v>
       </c>
-      <c r="L150" t="s">
+      <c r="L150" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M150" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N150" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="O150" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P150">
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>87</v>
       </c>
@@ -9956,23 +9955,23 @@
       <c r="K151" t="s">
         <v>465</v>
       </c>
-      <c r="L151" t="s">
+      <c r="L151" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M151" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N151" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="O151" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P151">
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>118</v>
       </c>
@@ -10006,23 +10005,23 @@
       <c r="K152" t="s">
         <v>465</v>
       </c>
-      <c r="L152" t="s">
+      <c r="L152" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M152" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N152" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="O152" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P152">
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>119</v>
       </c>
@@ -10056,23 +10055,23 @@
       <c r="K153" t="s">
         <v>465</v>
       </c>
-      <c r="L153" t="s">
+      <c r="L153" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M153" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N153" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="O153" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P153">
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>120</v>
       </c>
@@ -10106,23 +10105,23 @@
       <c r="K154" t="s">
         <v>353</v>
       </c>
-      <c r="L154" t="s">
+      <c r="L154" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M154" t="s">
+        <v>483</v>
+      </c>
+      <c r="N154" t="s">
+        <v>545</v>
+      </c>
+      <c r="O154" t="s">
         <v>484</v>
       </c>
-      <c r="N154" t="s">
-        <v>546</v>
-      </c>
-      <c r="O154" t="s">
-        <v>485</v>
-      </c>
       <c r="P154">
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>53</v>
       </c>
@@ -10156,23 +10155,23 @@
       <c r="K155" t="s">
         <v>353</v>
       </c>
-      <c r="L155" t="s">
+      <c r="L155" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M155" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N155" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="O155" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P155">
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>40</v>
       </c>
@@ -10206,23 +10205,23 @@
       <c r="K156" t="s">
         <v>353</v>
       </c>
-      <c r="L156" t="s">
+      <c r="L156" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M156" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N156" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="O156" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P156">
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>121</v>
       </c>
@@ -10256,23 +10255,23 @@
       <c r="K157" t="s">
         <v>353</v>
       </c>
-      <c r="L157" t="s">
+      <c r="L157" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M157" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N157" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="O157" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="P157">
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>122</v>
       </c>
@@ -10306,23 +10305,23 @@
       <c r="K158" t="s">
         <v>473</v>
       </c>
-      <c r="L158" t="s">
+      <c r="L158" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M158" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N158" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="O158" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P158">
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>123</v>
       </c>
@@ -10356,23 +10355,23 @@
       <c r="K159" t="s">
         <v>473</v>
       </c>
-      <c r="L159" t="s">
+      <c r="L159" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M159" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N159" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="O159" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P159">
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>124</v>
       </c>
@@ -10406,23 +10405,23 @@
       <c r="K160" t="s">
         <v>473</v>
       </c>
-      <c r="L160" t="s">
+      <c r="L160" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M160" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N160" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O160" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P160">
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>125</v>
       </c>
@@ -10456,23 +10455,23 @@
       <c r="K161" t="s">
         <v>473</v>
       </c>
-      <c r="L161" t="s">
+      <c r="L161" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M161" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N161" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="O161" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P161">
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>122</v>
       </c>
@@ -10506,23 +10505,23 @@
       <c r="K162" t="s">
         <v>450</v>
       </c>
-      <c r="L162" t="s">
+      <c r="L162" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M162" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N162" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="O162" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P162">
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>126</v>
       </c>
@@ -10556,23 +10555,23 @@
       <c r="K163" t="s">
         <v>450</v>
       </c>
-      <c r="L163" t="s">
+      <c r="L163" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M163" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N163" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="O163" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P163">
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>127</v>
       </c>
@@ -10606,23 +10605,23 @@
       <c r="K164" t="s">
         <v>450</v>
       </c>
-      <c r="L164" t="s">
+      <c r="L164" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M164" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N164" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="O164" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P164">
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>128</v>
       </c>
@@ -10656,23 +10655,23 @@
       <c r="K165" t="s">
         <v>450</v>
       </c>
-      <c r="L165" t="s">
+      <c r="L165" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M165" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N165" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="O165" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P165">
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>30</v>
       </c>
@@ -10706,23 +10705,23 @@
       <c r="K166" t="s">
         <v>352</v>
       </c>
-      <c r="L166" t="s">
+      <c r="L166" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M166" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N166" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="O166" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P166">
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>52</v>
       </c>
@@ -10756,23 +10755,23 @@
       <c r="K167" t="s">
         <v>352</v>
       </c>
-      <c r="L167" t="s">
+      <c r="L167" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M167" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N167" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="O167" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P167">
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>129</v>
       </c>
@@ -10806,23 +10805,23 @@
       <c r="K168" t="s">
         <v>352</v>
       </c>
-      <c r="L168" t="s">
+      <c r="L168" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M168" t="s">
+        <v>483</v>
+      </c>
+      <c r="N168" t="s">
+        <v>636</v>
+      </c>
+      <c r="O168" t="s">
         <v>484</v>
       </c>
-      <c r="N168" t="s">
-        <v>637</v>
-      </c>
-      <c r="O168" t="s">
-        <v>485</v>
-      </c>
       <c r="P168">
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>130</v>
       </c>
@@ -10856,23 +10855,23 @@
       <c r="K169" t="s">
         <v>352</v>
       </c>
-      <c r="L169" t="s">
+      <c r="L169" s="11" t="s">
         <v>478</v>
       </c>
       <c r="M169" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N169" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="O169" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P169">
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>90</v>
       </c>
@@ -10907,22 +10906,22 @@
         <v>474</v>
       </c>
       <c r="L170" t="s">
+        <v>476</v>
+      </c>
+      <c r="M170" t="s">
         <v>481</v>
       </c>
-      <c r="M170" t="s">
-        <v>482</v>
-      </c>
       <c r="N170" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="O170" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P170">
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>80</v>
       </c>
@@ -10957,22 +10956,22 @@
         <v>474</v>
       </c>
       <c r="L171" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="M171" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N171" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="O171" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P171">
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>131</v>
       </c>
@@ -11007,22 +11006,22 @@
         <v>474</v>
       </c>
       <c r="L172" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="M172" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N172" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O172" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P172">
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>132</v>
       </c>
@@ -11057,23 +11056,30 @@
         <v>474</v>
       </c>
       <c r="L173" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="M173" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N173" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="O173" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P173">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P173" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:P173" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="Profesional / Analista"/>
+        <filter val="Profesional Contable"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11082,21 +11088,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A9EAA1-EB7F-45F3-BA80-95884B8E9BF8}">
   <dimension ref="B2:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="2"/>
-    <col min="2" max="2" width="27.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="11.5703125" style="2"/>
+    <col min="2" max="2" width="27.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>466</v>
       </c>
@@ -11110,7 +11116,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -11118,7 +11124,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
@@ -11128,7 +11134,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="4" t="s">
@@ -11136,7 +11142,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="4" t="s">
@@ -11144,7 +11150,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="4" t="s">
@@ -11154,7 +11160,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="4" t="s">
         <v>352</v>
@@ -11164,13 +11170,13 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>363</v>
       </c>
@@ -11180,7 +11186,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="4" t="s">
         <v>354</v>
@@ -11190,7 +11196,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="4" t="s">
         <v>367</v>
@@ -11198,7 +11204,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>455</v>
       </c>
@@ -11206,19 +11212,19 @@
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="3" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="3" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>457</v>
       </c>
@@ -11226,7 +11232,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>458</v>
       </c>
@@ -11234,7 +11240,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>459</v>
       </c>
@@ -11242,7 +11248,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>460</v>
       </c>
@@ -11250,7 +11256,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>437</v>
       </c>
@@ -11258,7 +11264,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>461</v>
       </c>
@@ -11266,7 +11272,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>462</v>
       </c>
@@ -11274,13 +11280,13 @@
         <v>447</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="3" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>463</v>
       </c>
@@ -11288,7 +11294,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>456</v>
       </c>
@@ -11296,7 +11302,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>464</v>
       </c>
@@ -11304,25 +11310,25 @@
         <v>350</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="3" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="C39" s="3" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="C40" s="3" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>465</v>
       </c>
@@ -11330,13 +11336,13 @@
         <v>449</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="3" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>467</v>
       </c>
@@ -11344,13 +11350,13 @@
         <v>359</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="C46" s="3" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>468</v>
       </c>
@@ -11358,7 +11364,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>469</v>
       </c>
@@ -11366,7 +11372,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>470</v>
       </c>
@@ -11374,7 +11380,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>471</v>
       </c>
@@ -11382,7 +11388,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>472</v>
       </c>
@@ -11390,7 +11396,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
         <v>473</v>
       </c>
@@ -11398,7 +11404,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>474</v>
       </c>

</xml_diff>

<commit_message>
feedback de Beatriz completo
</commit_message>
<xml_diff>
--- a/data/tst.xlsx
+++ b/data/tst.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft5167433-my.sharepoint.com/personal/mfuquene_tads_com_co/Documents/Escritorio/Organigrama KPIs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="13_ncr:1_{564F41E0-5813-4ECD-BBF4-BF08FE283E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB53413B-82FA-4D94-8CD8-49D86323883D}"/>
+  <xr:revisionPtr revIDLastSave="323" documentId="13_ncr:1_{564F41E0-5813-4ECD-BBF4-BF08FE283E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6439EE81-D2ED-424F-B96F-CDBC69C10B95}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" r:id="rId1"/>
@@ -2058,7 +2058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2090,7 +2090,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2395,11 +2394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F50" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50:L169"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2470,7 +2468,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2520,7 +2518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2570,7 +2568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2620,7 +2618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2670,7 +2668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2720,7 +2718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2770,7 +2768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2820,7 +2818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2870,7 +2868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2920,7 +2918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2970,7 +2968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -3020,7 +3018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3070,7 +3068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -3120,7 +3118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -3170,7 +3168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3220,7 +3218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -3270,7 +3268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -3320,7 +3318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -3370,7 +3368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -3420,7 +3418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -3470,7 +3468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -3520,7 +3518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3570,7 +3568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -3620,7 +3618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -3670,7 +3668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -3720,7 +3718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -3770,7 +3768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -3820,7 +3818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -3870,7 +3868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -3920,7 +3918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -3970,7 +3968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -4020,7 +4018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -4070,7 +4068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -4120,7 +4118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -4170,7 +4168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -4220,7 +4218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -4270,7 +4268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -4320,7 +4318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -4370,7 +4368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -4420,7 +4418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -4470,7 +4468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -4520,7 +4518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -4570,7 +4568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -4620,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -4670,7 +4668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -4720,7 +4718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -4770,7 +4768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -4820,7 +4818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -4904,7 +4902,7 @@
       <c r="K50" t="s">
         <v>464</v>
       </c>
-      <c r="L50" s="11" t="s">
+      <c r="L50" t="s">
         <v>478</v>
       </c>
       <c r="M50" t="s">
@@ -4954,7 +4952,7 @@
       <c r="K51" t="s">
         <v>464</v>
       </c>
-      <c r="L51" s="11" t="s">
+      <c r="L51" t="s">
         <v>478</v>
       </c>
       <c r="M51" t="s">
@@ -5004,7 +5002,7 @@
       <c r="K52" t="s">
         <v>464</v>
       </c>
-      <c r="L52" s="11" t="s">
+      <c r="L52" t="s">
         <v>478</v>
       </c>
       <c r="M52" t="s">
@@ -5054,7 +5052,7 @@
       <c r="K53" t="s">
         <v>464</v>
       </c>
-      <c r="L53" s="11" t="s">
+      <c r="L53" t="s">
         <v>478</v>
       </c>
       <c r="M53" t="s">
@@ -5104,7 +5102,7 @@
       <c r="K54" t="s">
         <v>465</v>
       </c>
-      <c r="L54" s="11" t="s">
+      <c r="L54" t="s">
         <v>478</v>
       </c>
       <c r="M54" t="s">
@@ -5154,7 +5152,7 @@
       <c r="K55" t="s">
         <v>465</v>
       </c>
-      <c r="L55" s="11" t="s">
+      <c r="L55" t="s">
         <v>478</v>
       </c>
       <c r="M55" t="s">
@@ -5204,7 +5202,7 @@
       <c r="K56" t="s">
         <v>465</v>
       </c>
-      <c r="L56" s="11" t="s">
+      <c r="L56" t="s">
         <v>478</v>
       </c>
       <c r="M56" t="s">
@@ -5254,7 +5252,7 @@
       <c r="K57" t="s">
         <v>465</v>
       </c>
-      <c r="L57" s="11" t="s">
+      <c r="L57" t="s">
         <v>478</v>
       </c>
       <c r="M57" t="s">
@@ -5270,7 +5268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -5320,7 +5318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -5370,7 +5368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -5420,7 +5418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -5470,7 +5468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -5520,7 +5518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>39</v>
       </c>
@@ -5570,7 +5568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -5620,7 +5618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>40</v>
       </c>
@@ -5670,7 +5668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -5720,7 +5718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -5770,7 +5768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>47</v>
       </c>
@@ -5820,7 +5818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -5870,7 +5868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -5920,7 +5918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -5970,7 +5968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -6020,7 +6018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -6070,7 +6068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -6120,7 +6118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -6170,7 +6168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>40</v>
       </c>
@@ -6220,7 +6218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -6270,7 +6268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -6320,7 +6318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>75</v>
       </c>
@@ -6370,7 +6368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -6420,7 +6418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -6470,7 +6468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -6520,7 +6518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -6570,7 +6568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -6620,7 +6618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -6704,7 +6702,7 @@
       <c r="K86" t="s">
         <v>353</v>
       </c>
-      <c r="L86" s="11" t="s">
+      <c r="L86" t="s">
         <v>478</v>
       </c>
       <c r="M86" t="s">
@@ -6754,7 +6752,7 @@
       <c r="K87" t="s">
         <v>353</v>
       </c>
-      <c r="L87" s="11" t="s">
+      <c r="L87" t="s">
         <v>478</v>
       </c>
       <c r="M87" t="s">
@@ -6804,7 +6802,7 @@
       <c r="K88" t="s">
         <v>353</v>
       </c>
-      <c r="L88" s="11" t="s">
+      <c r="L88" t="s">
         <v>478</v>
       </c>
       <c r="M88" t="s">
@@ -6854,7 +6852,7 @@
       <c r="K89" t="s">
         <v>353</v>
       </c>
-      <c r="L89" s="11" t="s">
+      <c r="L89" t="s">
         <v>478</v>
       </c>
       <c r="M89" t="s">
@@ -6870,7 +6868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>83</v>
       </c>
@@ -6920,7 +6918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>84</v>
       </c>
@@ -6970,7 +6968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>85</v>
       </c>
@@ -7020,7 +7018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>86</v>
       </c>
@@ -7070,7 +7068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>74</v>
       </c>
@@ -7120,7 +7118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>79</v>
       </c>
@@ -7170,7 +7168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>40</v>
       </c>
@@ -7220,7 +7218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>78</v>
       </c>
@@ -7270,7 +7268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>61</v>
       </c>
@@ -7320,7 +7318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -7370,7 +7368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>88</v>
       </c>
@@ -7420,7 +7418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>89</v>
       </c>
@@ -7470,7 +7468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -7520,7 +7518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>91</v>
       </c>
@@ -7570,7 +7568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>92</v>
       </c>
@@ -7620,7 +7618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>93</v>
       </c>
@@ -7670,7 +7668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>94</v>
       </c>
@@ -7720,7 +7718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>95</v>
       </c>
@@ -7770,7 +7768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>96</v>
       </c>
@@ -7820,7 +7818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>70</v>
       </c>
@@ -7870,7 +7868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>83</v>
       </c>
@@ -7920,7 +7918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>97</v>
       </c>
@@ -7970,7 +7968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>75</v>
       </c>
@@ -8020,7 +8018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>86</v>
       </c>
@@ -8104,7 +8102,7 @@
       <c r="K114" t="s">
         <v>467</v>
       </c>
-      <c r="L114" s="11" t="s">
+      <c r="L114" t="s">
         <v>478</v>
       </c>
       <c r="M114" t="s">
@@ -8154,7 +8152,7 @@
       <c r="K115" t="s">
         <v>467</v>
       </c>
-      <c r="L115" s="11" t="s">
+      <c r="L115" t="s">
         <v>478</v>
       </c>
       <c r="M115" t="s">
@@ -8204,7 +8202,7 @@
       <c r="K116" t="s">
         <v>467</v>
       </c>
-      <c r="L116" s="11" t="s">
+      <c r="L116" t="s">
         <v>478</v>
       </c>
       <c r="M116" t="s">
@@ -8254,7 +8252,7 @@
       <c r="K117" t="s">
         <v>467</v>
       </c>
-      <c r="L117" s="11" t="s">
+      <c r="L117" t="s">
         <v>478</v>
       </c>
       <c r="M117" t="s">
@@ -8304,7 +8302,7 @@
       <c r="K118" t="s">
         <v>464</v>
       </c>
-      <c r="L118" s="11" t="s">
+      <c r="L118" t="s">
         <v>478</v>
       </c>
       <c r="M118" t="s">
@@ -8354,7 +8352,7 @@
       <c r="K119" t="s">
         <v>464</v>
       </c>
-      <c r="L119" s="11" t="s">
+      <c r="L119" t="s">
         <v>478</v>
       </c>
       <c r="M119" t="s">
@@ -8404,7 +8402,7 @@
       <c r="K120" t="s">
         <v>464</v>
       </c>
-      <c r="L120" s="11" t="s">
+      <c r="L120" t="s">
         <v>478</v>
       </c>
       <c r="M120" t="s">
@@ -8454,7 +8452,7 @@
       <c r="K121" t="s">
         <v>464</v>
       </c>
-      <c r="L121" s="11" t="s">
+      <c r="L121" t="s">
         <v>478</v>
       </c>
       <c r="M121" t="s">
@@ -8504,7 +8502,7 @@
       <c r="K122" t="s">
         <v>464</v>
       </c>
-      <c r="L122" s="11" t="s">
+      <c r="L122" t="s">
         <v>478</v>
       </c>
       <c r="M122" t="s">
@@ -8554,7 +8552,7 @@
       <c r="K123" t="s">
         <v>464</v>
       </c>
-      <c r="L123" s="11" t="s">
+      <c r="L123" t="s">
         <v>478</v>
       </c>
       <c r="M123" t="s">
@@ -8604,7 +8602,7 @@
       <c r="K124" t="s">
         <v>464</v>
       </c>
-      <c r="L124" s="11" t="s">
+      <c r="L124" t="s">
         <v>478</v>
       </c>
       <c r="M124" t="s">
@@ -8654,7 +8652,7 @@
       <c r="K125" t="s">
         <v>437</v>
       </c>
-      <c r="L125" s="11" t="s">
+      <c r="L125" t="s">
         <v>478</v>
       </c>
       <c r="M125" t="s">
@@ -8704,7 +8702,7 @@
       <c r="K126" t="s">
         <v>464</v>
       </c>
-      <c r="L126" s="11" t="s">
+      <c r="L126" t="s">
         <v>478</v>
       </c>
       <c r="M126" t="s">
@@ -8754,7 +8752,7 @@
       <c r="K127" t="s">
         <v>464</v>
       </c>
-      <c r="L127" s="11" t="s">
+      <c r="L127" t="s">
         <v>478</v>
       </c>
       <c r="M127" t="s">
@@ -8804,7 +8802,7 @@
       <c r="K128" t="s">
         <v>464</v>
       </c>
-      <c r="L128" s="11" t="s">
+      <c r="L128" t="s">
         <v>478</v>
       </c>
       <c r="M128" t="s">
@@ -8854,7 +8852,7 @@
       <c r="K129" t="s">
         <v>464</v>
       </c>
-      <c r="L129" s="11" t="s">
+      <c r="L129" t="s">
         <v>478</v>
       </c>
       <c r="M129" t="s">
@@ -8904,7 +8902,7 @@
       <c r="K130" t="s">
         <v>462</v>
       </c>
-      <c r="L130" s="11" t="s">
+      <c r="L130" t="s">
         <v>478</v>
       </c>
       <c r="M130" t="s">
@@ -8954,7 +8952,7 @@
       <c r="K131" t="s">
         <v>462</v>
       </c>
-      <c r="L131" s="11" t="s">
+      <c r="L131" t="s">
         <v>478</v>
       </c>
       <c r="M131" t="s">
@@ -9004,7 +9002,7 @@
       <c r="K132" t="s">
         <v>462</v>
       </c>
-      <c r="L132" s="11" t="s">
+      <c r="L132" t="s">
         <v>478</v>
       </c>
       <c r="M132" t="s">
@@ -9054,7 +9052,7 @@
       <c r="K133" t="s">
         <v>462</v>
       </c>
-      <c r="L133" s="11" t="s">
+      <c r="L133" t="s">
         <v>478</v>
       </c>
       <c r="M133" t="s">
@@ -9104,7 +9102,7 @@
       <c r="K134" t="s">
         <v>470</v>
       </c>
-      <c r="L134" s="11" t="s">
+      <c r="L134" t="s">
         <v>478</v>
       </c>
       <c r="M134" t="s">
@@ -9154,7 +9152,7 @@
       <c r="K135" t="s">
         <v>470</v>
       </c>
-      <c r="L135" s="11" t="s">
+      <c r="L135" t="s">
         <v>478</v>
       </c>
       <c r="M135" t="s">
@@ -9204,7 +9202,7 @@
       <c r="K136" t="s">
         <v>470</v>
       </c>
-      <c r="L136" s="11" t="s">
+      <c r="L136" t="s">
         <v>478</v>
       </c>
       <c r="M136" t="s">
@@ -9254,7 +9252,7 @@
       <c r="K137" t="s">
         <v>470</v>
       </c>
-      <c r="L137" s="11" t="s">
+      <c r="L137" t="s">
         <v>478</v>
       </c>
       <c r="M137" t="s">
@@ -9304,7 +9302,7 @@
       <c r="K138" t="s">
         <v>455</v>
       </c>
-      <c r="L138" s="11" t="s">
+      <c r="L138" t="s">
         <v>478</v>
       </c>
       <c r="M138" t="s">
@@ -9354,7 +9352,7 @@
       <c r="K139" t="s">
         <v>455</v>
       </c>
-      <c r="L139" s="11" t="s">
+      <c r="L139" t="s">
         <v>478</v>
       </c>
       <c r="M139" t="s">
@@ -9404,7 +9402,7 @@
       <c r="K140" t="s">
         <v>455</v>
       </c>
-      <c r="L140" s="11" t="s">
+      <c r="L140" t="s">
         <v>478</v>
       </c>
       <c r="M140" t="s">
@@ -9454,7 +9452,7 @@
       <c r="K141" t="s">
         <v>455</v>
       </c>
-      <c r="L141" s="11" t="s">
+      <c r="L141" t="s">
         <v>478</v>
       </c>
       <c r="M141" t="s">
@@ -9504,7 +9502,7 @@
       <c r="K142" t="s">
         <v>471</v>
       </c>
-      <c r="L142" s="11" t="s">
+      <c r="L142" t="s">
         <v>478</v>
       </c>
       <c r="M142" t="s">
@@ -9554,7 +9552,7 @@
       <c r="K143" t="s">
         <v>471</v>
       </c>
-      <c r="L143" s="11" t="s">
+      <c r="L143" t="s">
         <v>478</v>
       </c>
       <c r="M143" t="s">
@@ -9604,7 +9602,7 @@
       <c r="K144" t="s">
         <v>471</v>
       </c>
-      <c r="L144" s="11" t="s">
+      <c r="L144" t="s">
         <v>478</v>
       </c>
       <c r="M144" t="s">
@@ -9654,7 +9652,7 @@
       <c r="K145" t="s">
         <v>471</v>
       </c>
-      <c r="L145" s="11" t="s">
+      <c r="L145" t="s">
         <v>478</v>
       </c>
       <c r="M145" t="s">
@@ -9704,7 +9702,7 @@
       <c r="K146" t="s">
         <v>472</v>
       </c>
-      <c r="L146" s="11" t="s">
+      <c r="L146" t="s">
         <v>478</v>
       </c>
       <c r="M146" t="s">
@@ -9754,7 +9752,7 @@
       <c r="K147" t="s">
         <v>472</v>
       </c>
-      <c r="L147" s="11" t="s">
+      <c r="L147" t="s">
         <v>478</v>
       </c>
       <c r="M147" t="s">
@@ -9805,7 +9803,7 @@
       <c r="K148" t="s">
         <v>472</v>
       </c>
-      <c r="L148" s="11" t="s">
+      <c r="L148" t="s">
         <v>478</v>
       </c>
       <c r="M148" t="s">
@@ -9855,7 +9853,7 @@
       <c r="K149" t="s">
         <v>472</v>
       </c>
-      <c r="L149" s="11" t="s">
+      <c r="L149" t="s">
         <v>478</v>
       </c>
       <c r="M149" t="s">
@@ -9905,7 +9903,7 @@
       <c r="K150" t="s">
         <v>465</v>
       </c>
-      <c r="L150" s="11" t="s">
+      <c r="L150" t="s">
         <v>478</v>
       </c>
       <c r="M150" t="s">
@@ -9955,7 +9953,7 @@
       <c r="K151" t="s">
         <v>465</v>
       </c>
-      <c r="L151" s="11" t="s">
+      <c r="L151" t="s">
         <v>478</v>
       </c>
       <c r="M151" t="s">
@@ -10005,7 +10003,7 @@
       <c r="K152" t="s">
         <v>465</v>
       </c>
-      <c r="L152" s="11" t="s">
+      <c r="L152" t="s">
         <v>478</v>
       </c>
       <c r="M152" t="s">
@@ -10055,7 +10053,7 @@
       <c r="K153" t="s">
         <v>465</v>
       </c>
-      <c r="L153" s="11" t="s">
+      <c r="L153" t="s">
         <v>478</v>
       </c>
       <c r="M153" t="s">
@@ -10105,7 +10103,7 @@
       <c r="K154" t="s">
         <v>353</v>
       </c>
-      <c r="L154" s="11" t="s">
+      <c r="L154" t="s">
         <v>478</v>
       </c>
       <c r="M154" t="s">
@@ -10155,7 +10153,7 @@
       <c r="K155" t="s">
         <v>353</v>
       </c>
-      <c r="L155" s="11" t="s">
+      <c r="L155" t="s">
         <v>478</v>
       </c>
       <c r="M155" t="s">
@@ -10205,7 +10203,7 @@
       <c r="K156" t="s">
         <v>353</v>
       </c>
-      <c r="L156" s="11" t="s">
+      <c r="L156" t="s">
         <v>478</v>
       </c>
       <c r="M156" t="s">
@@ -10255,7 +10253,7 @@
       <c r="K157" t="s">
         <v>353</v>
       </c>
-      <c r="L157" s="11" t="s">
+      <c r="L157" t="s">
         <v>478</v>
       </c>
       <c r="M157" t="s">
@@ -10305,7 +10303,7 @@
       <c r="K158" t="s">
         <v>473</v>
       </c>
-      <c r="L158" s="11" t="s">
+      <c r="L158" t="s">
         <v>478</v>
       </c>
       <c r="M158" t="s">
@@ -10355,7 +10353,7 @@
       <c r="K159" t="s">
         <v>473</v>
       </c>
-      <c r="L159" s="11" t="s">
+      <c r="L159" t="s">
         <v>478</v>
       </c>
       <c r="M159" t="s">
@@ -10405,7 +10403,7 @@
       <c r="K160" t="s">
         <v>473</v>
       </c>
-      <c r="L160" s="11" t="s">
+      <c r="L160" t="s">
         <v>478</v>
       </c>
       <c r="M160" t="s">
@@ -10455,7 +10453,7 @@
       <c r="K161" t="s">
         <v>473</v>
       </c>
-      <c r="L161" s="11" t="s">
+      <c r="L161" t="s">
         <v>478</v>
       </c>
       <c r="M161" t="s">
@@ -10505,7 +10503,7 @@
       <c r="K162" t="s">
         <v>450</v>
       </c>
-      <c r="L162" s="11" t="s">
+      <c r="L162" t="s">
         <v>478</v>
       </c>
       <c r="M162" t="s">
@@ -10555,7 +10553,7 @@
       <c r="K163" t="s">
         <v>450</v>
       </c>
-      <c r="L163" s="11" t="s">
+      <c r="L163" t="s">
         <v>478</v>
       </c>
       <c r="M163" t="s">
@@ -10605,7 +10603,7 @@
       <c r="K164" t="s">
         <v>450</v>
       </c>
-      <c r="L164" s="11" t="s">
+      <c r="L164" t="s">
         <v>478</v>
       </c>
       <c r="M164" t="s">
@@ -10655,7 +10653,7 @@
       <c r="K165" t="s">
         <v>450</v>
       </c>
-      <c r="L165" s="11" t="s">
+      <c r="L165" t="s">
         <v>478</v>
       </c>
       <c r="M165" t="s">
@@ -10705,7 +10703,7 @@
       <c r="K166" t="s">
         <v>352</v>
       </c>
-      <c r="L166" s="11" t="s">
+      <c r="L166" t="s">
         <v>478</v>
       </c>
       <c r="M166" t="s">
@@ -10755,7 +10753,7 @@
       <c r="K167" t="s">
         <v>352</v>
       </c>
-      <c r="L167" s="11" t="s">
+      <c r="L167" t="s">
         <v>478</v>
       </c>
       <c r="M167" t="s">
@@ -10805,7 +10803,7 @@
       <c r="K168" t="s">
         <v>352</v>
       </c>
-      <c r="L168" s="11" t="s">
+      <c r="L168" t="s">
         <v>478</v>
       </c>
       <c r="M168" t="s">
@@ -10855,7 +10853,7 @@
       <c r="K169" t="s">
         <v>352</v>
       </c>
-      <c r="L169" s="11" t="s">
+      <c r="L169" t="s">
         <v>478</v>
       </c>
       <c r="M169" t="s">
@@ -10871,7 +10869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>90</v>
       </c>
@@ -10921,7 +10919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>80</v>
       </c>
@@ -10971,7 +10969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>131</v>
       </c>
@@ -11021,7 +11019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>132</v>
       </c>
@@ -11072,14 +11070,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P173" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="Profesional / Analista"/>
-        <filter val="Profesional Contable"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P173" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>